<commit_message>
Correction des bugs sur end_repeat, select et la feuille survey :version 1.0.3
</commit_message>
<xml_diff>
--- a/form.xlsx
+++ b/form.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="suvrey" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="choices" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="survey" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -539,17 +539,6 @@
  &lt;br&gt;
  L'objectif de l'étude est d'identifier les contraintes majeures à l'adoption des technologies et innovations 
  dans le domaine agricole, afin de proposer une stratégie de diffusion optimisant leur adoption. _note
- Objectifs spécifiques:
- Plus spécifiquement, il s'agira de : 
- - évaluer les principaux mécanismes de génération et de transferts d'innovations et de bonnes pratiques agricoles ; 
- - identifier les contraintes rencontrées dans le transfert et l'adoption des technologies et innovations ; 
- - proposer des solutions pour améliorer le transfert et l'adoption des innovations dans le contexte des systèmes de production ivoirien.
- &lt;br&gt;
- &lt;b&gt;Resultat attendu:&lt;/b&gt;
- Au terme de l'étude, les résultats attendus sont : 
- - un rapport est produit décrivant les mécanismes de génération et transfert des innovations 
- - des propositions pertinentes pour optimiser la diffusion et l'adoption des innovations 
- - les conclusions de l'étude sont restituées aux parties prenantes 
 </t>
         </is>
       </c>
@@ -748,7 +737,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>select_one choix_A_6</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -774,7 +763,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>select_one choix_A_7</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1174,7 +1163,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Si oui, quelles ont été les structures de diffusion ? $si</t>
+          <t>Si oui, quelles ont été les structures de diffusion ?</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -1204,7 +1193,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>B.2 En général comment appréciez-vous les interventions de ces structures ?</t>
+          <t xml:space="preserve">B.2 En général comment appréciez-vous les interventions de ces structures ? </t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
@@ -1224,7 +1213,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>select_one choix_B_table-1_1_0</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1250,7 +1239,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>select_one choix_B_table-1_1_1</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1276,7 +1265,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>select_one choix_B_table-1_1_2</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1302,7 +1291,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>select_one choix_B_table-1_1_3</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1328,7 +1317,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>select_one choix_B_table-1_1_4</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1354,7 +1343,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>select_one choix_B_table-1_1_5</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1450,7 +1439,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>select_multiple choix_B_5</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1460,7 +1449,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>B.5 Si oui, dans quel cadre ? $[ Votre OPA , Consultation individuelle] $si</t>
+          <t>B.5 Si oui, dans quel cadre ?</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
@@ -1506,7 +1495,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>end_repeat</t>
+          <t>end_group</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1587,7 +1576,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nature de l'innovation dont vous avez bénéficié. </t>
+          <t xml:space="preserve">C.1 Nature de l'innovation dont vous avez bénéficié. </t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
@@ -1603,7 +1592,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>date</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1613,7 +1602,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>C.2	Période de diffusion</t>
+          <t>C.2      Période de diffusion</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
@@ -1639,7 +1628,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t xml:space="preserve">C.3	Difficultés rencontrées pendant l'adoption	</t>
+          <t xml:space="preserve">C.3      Difficultés rencontrées pendant l'adoption      </t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
@@ -1655,7 +1644,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>select_one choix_C_4</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1665,7 +1654,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve">C.4	Maîtrise de l'innovation à ce jour </t>
+          <t xml:space="preserve">C.4      Maîtrise de l'innovation à ce jour </t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
@@ -1681,7 +1670,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>select_one choix_C_5</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1691,7 +1680,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t xml:space="preserve">C.5	Si peu ou pas maîtrisée, quelles sont les causes ? </t>
+          <t xml:space="preserve">C.5      Si peu ou pas maîtrisée, quelles sont les causes ? </t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
@@ -1733,7 +1722,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>select_one choix_C_6</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1829,7 +1818,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>select_one choix_D_1</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1839,7 +1828,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>D.1 .Pouvez-vous évaluer le niveau de pertinence de l'Innovation &amp; technologie ? _s1 $[Très pertinent,	pertinent,	Peu pertinent,	Pas pertinent	NSP]</t>
+          <t>D.1 .Pouvez-vous évaluer le niveau de pertinence de l'Innovation &amp; technologie ?</t>
         </is>
       </c>
       <c r="D53" t="inlineStr"/>
@@ -1865,7 +1854,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>D.2. Globalement Pensez-vous que l'innovation répondait à vos besoins ? _s1</t>
+          <t>D.2. Globalement Pensez-vous que l'innovation répondait à vos besoins ?</t>
         </is>
       </c>
       <c r="D54" t="inlineStr"/>
@@ -1987,7 +1976,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t xml:space="preserve">E.1	Si l'innovations a quelque peu répondu à vos besoins, quel impact sur votre activité ? </t>
+          <t xml:space="preserve">E.1      Si l'innovations a quelque peu répondu à vos besoins, quel impact sur votre activité ? : Detail pour Gain de productivité </t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2099,7 +2088,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t xml:space="preserve">E.1	Si l'innovations a quelque peu répondu à vos besoins, quel impact sur votre activité ? </t>
+          <t xml:space="preserve">E.1      Si l'innovations a quelque peu répondu à vos besoins, quel impact sur votre activité ? : Detail pour Gain de qualité </t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2211,7 +2200,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t xml:space="preserve">E.1	Si l'innovations a quelque peu répondu à vos besoins, quel impact sur votre activité ? </t>
+          <t xml:space="preserve">E.1      Si l'innovations a quelque peu répondu à vos besoins, quel impact sur votre activité ? : Detail pour Gain de temps </t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2323,7 +2312,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t xml:space="preserve">E.1	Si l'innovations a quelque peu répondu à vos besoins, quel impact sur votre activité ? </t>
+          <t xml:space="preserve">E.1      Si l'innovations a quelque peu répondu à vos besoins, quel impact sur votre activité ? : Detail pour Gain de revenu supplémentaire </t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2435,7 +2424,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t xml:space="preserve">E.1	Si l'innovations a quelque peu répondu à vos besoins, quel impact sur votre activité ? </t>
+          <t xml:space="preserve">E.1      Si l'innovations a quelque peu répondu à vos besoins, quel impact sur votre activité ? : Detail pour Autre impact sur votre activité </t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2565,7 +2554,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>F	EVALUATION DU MECANISME DE TRANSFERT DES INNOVATIONS GENEREES A LA VULGARISATION ET DE LA DURABILITE</t>
+          <t>F    EVALUATION DU MECANISME DE TRANSFERT DES INNOVATIONS GENEREES A LA VULGARISATION ET DE LA DURABILITE</t>
         </is>
       </c>
       <c r="D80" t="inlineStr"/>
@@ -2591,7 +2580,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t xml:space="preserve">F.1	L'innovation part du chercheur au vulgarisateur. Comment passe-t-elle du vulgarisateur à vous? </t>
+          <t xml:space="preserve">F.1      L'innovation part du chercheur au vulgarisateur. Comment passe-t-elle du vulgarisateur à vous? </t>
         </is>
       </c>
       <c r="D81" t="inlineStr"/>
@@ -2617,7 +2606,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>F.2	Avez-vous noté quelques difficultés de la diffusion de l'innovation?</t>
+          <t>F.2     Avez-vous noté quelques difficultés de la diffusion de l'innovation?</t>
         </is>
       </c>
       <c r="D82" t="inlineStr"/>
@@ -2669,7 +2658,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>F.3	Rencontrez-vous des difficultés à maintenir l'innovation dans votre activité ?</t>
+          <t>F.3     Rencontrez-vous des difficultés à maintenir l'innovation dans votre activité ?</t>
         </is>
       </c>
       <c r="D84" t="inlineStr"/>
@@ -2791,7 +2780,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t xml:space="preserve">G.1	Au vu de tout ce qui précède, quelles recommandations pouvez-vous faire pour l'amélioration du mécanisme de diffusion et de transfert des innovations aux bénéficiaires ? </t>
+          <t xml:space="preserve">G.1      Au vu de tout ce qui précède, quelles recommandations pouvez-vous faire pour l'amélioration du mécanisme de diffusion et de transfert des innovations aux bénéficiaires ? </t>
         </is>
       </c>
       <c r="D89" t="inlineStr"/>
@@ -2817,7 +2806,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>G.2	Selon vous, que faut-il faire pour que les innovations ne soient pas abandonnées après leur adoption par vous après un moment donné ?</t>
+          <t>G.2      Selon vous, que faut-il faire pour que les innovations ne soient pas abandonnées après leur adoption par vous après un moment donné ?</t>
         </is>
       </c>
       <c r="D90" t="inlineStr"/>
@@ -2843,7 +2832,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t xml:space="preserve">G.3	Que recommandez-vous au FCIAD pour pérenniser ses activités de transfert d'innovation et de technologies ? </t>
+          <t xml:space="preserve">G.3      Que recommandez-vous au FCIAD pour pérenniser ses activités de transfert d'innovation et de technologies ? </t>
         </is>
       </c>
       <c r="D91" t="inlineStr"/>
@@ -3137,7 +3126,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3195,7 +3184,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_A_6</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -3210,7 +3199,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_A_6</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -3225,7 +3214,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_A_6</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -3240,7 +3229,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_A_6</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -3255,7 +3244,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_A_6</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -3270,7 +3259,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_A_7</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -3285,7 +3274,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_A_7</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -3300,7 +3289,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_A_7</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -3315,7 +3304,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_A_7</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -3330,7 +3319,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_A_7</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -3345,7 +3334,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_A_7</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -3675,7 +3664,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_B_table-1_1_0</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -3690,7 +3679,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_B_table-1_1_0</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -3705,7 +3694,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_B_table-1_1_0</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -3720,7 +3709,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_B_table-1_1_0</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -3735,7 +3724,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>choix_B_4</t>
+          <t>choix_B_table-1_1_1</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -3743,14 +3732,14 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Oui</t>
+          <t>Très satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>choix_B_4</t>
+          <t>choix_B_table-1_1_1</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -3758,104 +3747,104 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Non</t>
+          <t xml:space="preserve"> Satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>choix_C_1</t>
+          <t>choix_B_table-1_1_1</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>C.1	Production</t>
+          <t xml:space="preserve"> Peu satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>choix_C_1</t>
+          <t>choix_B_table-1_1_1</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Transformation</t>
+          <t xml:space="preserve"> Pas du tout satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>choix_C_1</t>
+          <t>choix_B_table-1_1_2</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Valorisation</t>
+          <t>Très satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_B_table-1_1_2</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Formation insuffisante</t>
+          <t xml:space="preserve"> Satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_B_table-1_1_2</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ressources matérielles insuffisantes</t>
+          <t xml:space="preserve"> Peu satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_B_table-1_1_2</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Autre</t>
+          <t xml:space="preserve"> Pas du tout satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_B_table-1_1_3</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -3863,14 +3852,14 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Mois</t>
+          <t>Très satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_B_table-1_1_3</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -3878,14 +3867,14 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Campagnes</t>
+          <t xml:space="preserve"> Satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_B_table-1_1_3</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -3893,215 +3882,590 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Années</t>
+          <t xml:space="preserve"> Peu satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_B_table-1_1_3</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Très pertinent</t>
+          <t xml:space="preserve"> Pas du tout satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_B_table-1_1_4</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t xml:space="preserve">	pertinent</t>
+          <t>Très satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_B_table-1_1_4</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t xml:space="preserve">	Peu pertinent</t>
+          <t xml:space="preserve"> Satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>choix_B_table-1_1_4</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t xml:space="preserve">	Pas pertinent	NSP</t>
+          <t xml:space="preserve"> Peu satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>choix_D_2</t>
+          <t>choix_B_table-1_1_4</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Oui</t>
+          <t xml:space="preserve"> Pas du tout satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>choix_D_2</t>
+          <t>choix_B_table-1_1_5</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Non</t>
+          <t>Très satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>choix_D_3</t>
+          <t>choix_B_table-1_1_5</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>introduit peu de changement sur l'exploitation</t>
+          <t xml:space="preserve"> Satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>choix_D_3</t>
+          <t>choix_B_table-1_1_5</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>permet de résoudre un problème sectoriel et a des répercussions sur l'ensemble de l'exploitation</t>
+          <t xml:space="preserve"> Peu satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>choix_D_3</t>
+          <t>choix_B_table-1_1_5</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>implique l'adoption simultanée de diverses techniques cohérentes entre elles</t>
+          <t xml:space="preserve"> Pas du tout satisfaisant</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>choix_D_3</t>
+          <t>choix_B_4</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Autre</t>
+          <t>Oui</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>choix_F_2</t>
+          <t>choix_B_4</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Oui</t>
+          <t>Non</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>choix_F_2</t>
+          <t>choix_B_5</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Non</t>
+          <t xml:space="preserve">Votre OPA </t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>choix_F_3</t>
+          <t>choix_B_5</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Oui</t>
+          <t xml:space="preserve"> Consultation individuelle</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
+          <t>choix_C_1</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Production</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>choix_C_1</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>2</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Transformation</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>choix_C_1</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>3</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Valorisation</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>choix_C_4</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>1</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Bien maîtrisée</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>choix_C_4</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>2</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Peu maîtrisée</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>choix_C_4</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>3</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Pas encore maîtrisée</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>choix_C_5</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>1</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Formation insuffisante</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>choix_C_5</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>2</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ressources matérielles insuffisantes</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>choix_C_5</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>3</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Autre</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>choix_C_6</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Mois</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>choix_C_6</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>2</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Campagnes</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>choix_C_6</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>3</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Années</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>choix_D_1</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>1</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Très pertinent</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>choix_D_1</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>2</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> pertinent</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>choix_D_1</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>3</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      Peu pertinent</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>choix_D_1</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>4</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Pas pertinent   NSP</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>choix_D_2</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>1</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>choix_D_2</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>2</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Non</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>choix_D_3</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>1</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>introduit peu de changement sur l'exploitation</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>choix_D_3</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>2</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>permet de résoudre un problème sectoriel et a des répercussions sur l'ensemble de l'exploitation</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>choix_D_3</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>3</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>implique l'adoption simultanée de diverses techniques cohérentes entre elles</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>choix_D_3</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>4</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Autre</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>choix_F_2</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>1</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>choix_F_2</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>2</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Non</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
           <t>choix_F_3</t>
         </is>
       </c>
-      <c r="B64" t="n">
+      <c r="B88" t="n">
+        <v>1</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>choix_F_3</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
         <v>2</v>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="C89" t="inlineStr">
         <is>
           <t>Non</t>
         </is>

</xml_diff>

<commit_message>
Gestion des regex complexe
</commit_message>
<xml_diff>
--- a/form.xlsx
+++ b/form.xlsx
@@ -477,7 +477,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>constarint_message</t>
+          <t>constraint_message</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -678,7 +678,11 @@
       </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>regex(.,"[A-ZÀ-ÖØ-ÞĀĂĄĆĈĊČĎĐĒĔĖĘĚĜĞĠĢĤĦĨĪĬĮİĲĴĶĹĻĽĿŁŃŅŇŊŌŎŐŒŔŖŘŚŜŞŠŢŤŦŨŪŬŮŰŲŴŶŸ-ŹŻŽƁ-ƂƄƆ-ƇƉ-ƋƎ-ƑƓ-ƔƖ-ƘƜ-ƝƟ-ƠƢƤƦ-ƧƩƬƮ-ƯƱ-ƳƵƷ-ƸƼǄǇǊǍǏǑǓǕǗǙǛǞǠǢǤǦǨǪǬǮǱǴǶ-ǸǺǼǾȀȂȄȆȈȊȌȎȐȒȔȖȘȚȜȞȠȢȤȦȨȪȬȮȰȲȺ-ȻȽ-ȾɁɃ-ɆɈɊɌɎͰͲͶͿΆΈ-ΊΌΎ-ΏΑ-ΡΣ-ΫϏϒ-ϔϘϚϜϞϠϢϤϦϨϪϬϮϴϷϹ-ϺϽ-ЯѠѢѤѦѨѪѬѮѰѲѴѶѸѺѼѾҀҊҌҎҐҒҔҖҘҚҜҞҠҢҤҦҨҪҬҮҰҲҴҶҸҺҼҾӀ-ӁӃӅӇӉӋӍӐӒӔӖӘӚӜӞӠӢӤӦӨӪӬӮӰӲӴӶӸӺӼӾԀԂԄԆԈԊԌԎԐԒԔԖԘԚԜԞԠԢԤԦԨԪԬԮԱ-ՖႠ-ჅჇჍᎠ-ᏵᲐ-ᲺᲽ-ᲿḀḂḄḆḈḊḌḎḐḒḔḖḘḚḜḞḠḢḤḦḨḪḬḮḰḲḴḶḸḺḼḾṀṂṄṆṈṊṌṎṐṒṔṖṘṚṜṞṠṢṤṦṨṪṬṮṰṲṴṶṸṺṼṾẀẂẄẆẈẊẌẎẐẒẔẞẠẢẤẦẨẪẬẮẰẲẴẶẸẺẼẾỀỂỄỆỈỊỌỎỐỒỔỖỘỚỜỞỠỢỤỦỨỪỬỮỰỲỴỶỸỺỼỾἈ-ἏἘ-ἝἨ-ἯἸ-ἿὈ-ὍὙὛὝὟὨ-ὯᾸ-ΆῈ-ΉῘ-ΊῨ-ῬῸ-Ώℂℇℋ-ℍℐ-ℒℕℙ-ℝℤΩℨK-ℭℰ-ℳℾ-ℿⅅⅠ-ⅯↃⒶ-ⓏⰀ-ⰮⱠⱢ-ⱤⱧⱩⱫⱭ-ⱰⱲⱵⱾ-ⲀⲂⲄⲆⲈⲊⲌⲎⲐⲒⲔⲖⲘⲚⲜⲞⲠⲢⲤⲦⲨⲪⲬⲮⲰⲲⲴⲶⲸⲺⲼⲾⳀⳂⳄⳆⳈⳊⳌⳎⳐⳒⳔⳖⳘⳚⳜⳞⳠⳢⳫⳭⳲꙀꙂꙄꙆꙈꙊꙌꙎꙐꙒꙔꙖꙘꙚꙜꙞꙠꙢꙤꙦꙨꙪꙬꚀꚂꚄꚆꚈꚊꚌꚎꚐꚒꚔꚖꚘꚚꜢꜤꜦꜨꜪꜬꜮꜲꜴꜶꜸꜺꜼꜾꝀꝂꝄꝆꝈꝊꝌꝎꝐꝒꝔꝖꝘꝚꝜꝞꝠꝢꝤꝦꝨꝪꝬꝮꝹꝻꝽ-ꝾꞀꞂꞄꞆꞋꞍꞐꞒꞖꞘꞚꞜꞞꞠꞢꞤꞦꞨꞪ-ꞮꞰ-ꞴꞶꞸꞺꞼꞾꟂꟄ-ꟇꟉꟵＡ-Ｚ𐐀-𐐧𐒰-𐓓𐲀-𐲲𑢠-𑢿𖹀-𖹟𝐀-𝐙𝐴-𝑍𝑨-𝒁𝒜𝒞-𝒟𝒢𝒥-𝒦𝒩-𝒬𝒮-𝒵𝓐-𝓩𝔄-𝔅𝔇-𝔊𝔍-𝔔𝔖-𝔜𝔸-𝔹𝔻-𝔾𝕀-𝕄𝕆𝕊-𝕐𝕬-𝖅𝖠-𝖹𝗔-𝗭𝘈-𝘡𝘼-𝙕𝙰-𝚉𝚨-𝛀𝛢-𝛺𝜜-𝜴𝝖-𝝮𝞐-𝞨𝟊𞤀-𞤡🄰-🅉🅐-🅩🅰-🆉]{,2}")</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
@@ -697,7 +701,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>A.3 Prénoms **</t>
+          <t>A.3 Prénoms ** $=</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -706,7 +710,11 @@
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>regex(.,"^([a-z]{1,}(['])?[a-z]+)([ ][a-z]{1,}(['])?[a-z]+)+$")</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -888,7 +896,11 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>regex(.,"^(1|05|07)((?:[-]\d{2}){4}|(?:[ ]\d{2}){4}|\d{8})$")</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
@@ -914,7 +926,11 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>regex(.,"^[a-zA-Z0-9._%+-]+@[a-zA-Z0-9.-]+\.[a-zA-Z]{2,}$")</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
@@ -1490,7 +1506,7 @@
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>selected(${B_5},'autre'</t>
+          <t>${B_5}='autre'</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>

</xml_diff>